<commit_message>
continued work on validation plots
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F452A0A-FF07-5946-99F8-3F3E0A05B355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B69826-CF6C-1044-A769-69ACA2839475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="500" windowWidth="30760" windowHeight="19640" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="20420" yWindow="500" windowWidth="18280" windowHeight="19640" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="428">
   <si>
     <t>order</t>
   </si>
@@ -1286,6 +1286,45 @@
   </si>
   <si>
     <t>spread x axis wide as you get co-elution but shifted, possible matrix effect, showed full and curated peaks zoomed in on y, eliminated massive peak</t>
+  </si>
+  <si>
+    <t>shrunk y axis for sample</t>
+  </si>
+  <si>
+    <t>shrunk y axis for sample, removed mz0 to zoom on mz3</t>
+  </si>
+  <si>
+    <t>shrunk y axis</t>
+  </si>
+  <si>
+    <t>zoomed x and y</t>
+  </si>
+  <si>
+    <t>shrunk axes, eliminated mz0 and mz4 to show smaller fragments</t>
+  </si>
+  <si>
+    <t>zoomed to mz0 and zoomed y</t>
+  </si>
+  <si>
+    <t>zoomed x</t>
+  </si>
+  <si>
+    <t>copied and checking</t>
+  </si>
+  <si>
+    <t>zoomed x axis</t>
+  </si>
+  <si>
+    <t>zoomed x axis, zoomed to mz1</t>
+  </si>
+  <si>
+    <t>zoomed x axis, removed mz3</t>
+  </si>
+  <si>
+    <t>close look at all 6 just showed way too much noise and quant frag way too small</t>
+  </si>
+  <si>
+    <t>peaks that are being annotated are always a few seconds away from elution, very noisy, failing</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,6 +1364,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1356,7 +1401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1377,6 +1422,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1724,15 +1770,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K82" sqref="K82"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
@@ -1811,7 +1857,7 @@
       <c r="I2" s="2">
         <v>6.45</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1847,7 +1893,7 @@
       <c r="I3" s="2">
         <v>6.25</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -1883,7 +1929,7 @@
       <c r="I4" s="2">
         <v>6.55</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1921,7 +1967,7 @@
       <c r="I5" s="2">
         <v>13.85</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1959,10 +2005,12 @@
       <c r="I6" s="2">
         <v>7.9249999999999998</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>422</v>
+      </c>
       <c r="L6" s="2" t="s">
         <v>279</v>
       </c>
@@ -1995,7 +2043,7 @@
       <c r="I7" s="2">
         <v>13.45</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -2033,7 +2081,7 @@
       <c r="I8" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>343</v>
       </c>
       <c r="K8" s="2"/>
@@ -2069,7 +2117,7 @@
       <c r="I9" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>343</v>
       </c>
       <c r="K9" s="2"/>
@@ -2105,7 +2153,7 @@
       <c r="I10" s="2">
         <v>6.5</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -2141,7 +2189,7 @@
       <c r="I11" s="2">
         <v>6.5</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>340</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -2177,10 +2225,12 @@
       <c r="I12" s="2">
         <v>9.2249999999999996</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K12" s="2"/>
+      <c r="J12" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>416</v>
+      </c>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2211,10 +2261,12 @@
       <c r="I13" s="2">
         <v>9.7750000000000004</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K13" s="2"/>
+      <c r="J13" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>415</v>
+      </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2245,10 +2297,12 @@
       <c r="I14" s="2">
         <v>3.95</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K14" s="2"/>
+      <c r="J14" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>417</v>
+      </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2279,10 +2333,12 @@
       <c r="I15" s="2">
         <v>9.65</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K15" s="2"/>
+      <c r="J15" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>417</v>
+      </c>
       <c r="L15" s="2" t="s">
         <v>308</v>
       </c>
@@ -2315,10 +2371,12 @@
       <c r="I16" s="2">
         <v>11.3575</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K16" s="2"/>
+      <c r="J16" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>257</v>
       </c>
@@ -2351,10 +2409,12 @@
       <c r="I17" s="2">
         <v>22.45</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K17" s="2"/>
+      <c r="J17" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2385,10 +2445,12 @@
       <c r="I18" s="2">
         <v>9.65</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K18" s="2"/>
+      <c r="J18" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>420</v>
+      </c>
       <c r="L18" s="2" t="s">
         <v>242</v>
       </c>
@@ -2421,10 +2483,12 @@
       <c r="I19" s="2">
         <v>9.5500000000000007</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K19" s="2"/>
+      <c r="J19" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="L19" s="2" t="s">
         <v>243</v>
       </c>
@@ -2457,10 +2521,12 @@
       <c r="I20" s="2">
         <v>2.5</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K20" s="2"/>
+      <c r="J20" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2482,20 +2548,22 @@
       <c r="F21" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="3">
-        <v>1</v>
+      <c r="G21" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="H21" s="2">
-        <v>8.0250000000000004</v>
+        <v>13.425000000000001</v>
       </c>
       <c r="I21" s="2">
-        <v>8.25</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>329</v>
+        <v>13.574999999999999</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>343</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -2525,10 +2593,12 @@
       <c r="I22" s="2">
         <v>18.149999999999999</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K22" s="2"/>
+      <c r="J22" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>424</v>
+      </c>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2559,10 +2629,12 @@
       <c r="I23" s="2">
         <v>10.102499999999999</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K23" s="2"/>
+      <c r="J23" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>423</v>
+      </c>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2593,10 +2665,12 @@
       <c r="I24" s="2">
         <v>7.875</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K24" s="2"/>
+      <c r="J24" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>425</v>
+      </c>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2627,10 +2701,12 @@
       <c r="I25" s="2">
         <v>6.75</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K25" s="2"/>
+      <c r="J25" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>423</v>
+      </c>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2652,8 +2728,8 @@
       <c r="F26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G26" s="3">
-        <v>1</v>
+      <c r="G26" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="H26" s="2">
         <v>4.9000000000000004</v>
@@ -2661,11 +2737,13 @@
       <c r="I26" s="2">
         <v>5.05</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>329</v>
+      <c r="J26" s="10" t="s">
+        <v>343</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="L26" s="2" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -2695,10 +2773,12 @@
       <c r="I27" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="K27" s="2"/>
+      <c r="J27" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>423</v>
+      </c>
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2955,7 +3035,7 @@
       <c r="I34" s="2">
         <v>7.55</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K34" s="2"/>
@@ -2989,7 +3069,7 @@
       <c r="I35" s="2">
         <v>5.3</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K35" s="2"/>
@@ -3023,7 +3103,7 @@
       <c r="I36" s="2">
         <v>12.875</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K36" s="2"/>
@@ -3057,7 +3137,7 @@
       <c r="I37" s="2">
         <v>7.4</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K37" s="2"/>
@@ -3091,7 +3171,7 @@
       <c r="I38" s="2">
         <v>16.574999999999999</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K38" s="2"/>
@@ -3127,7 +3207,7 @@
       <c r="I39" s="2">
         <v>7.5250000000000004</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K39" s="2"/>
@@ -3163,7 +3243,7 @@
       <c r="I40" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K40" s="2"/>
@@ -3199,7 +3279,7 @@
       <c r="I41" s="2">
         <v>4.45</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K41" s="2"/>
@@ -3235,7 +3315,7 @@
       <c r="I42" s="2">
         <v>4.45</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K42" s="2"/>
@@ -3271,7 +3351,7 @@
       <c r="I43" s="2">
         <v>11.25</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K43" s="2"/>
@@ -3305,7 +3385,7 @@
       <c r="I44" s="2">
         <v>17.45</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K44" s="2"/>

</xml_diff>

<commit_message>
added back validation pdf compile fxn
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB9FB19-1838-C749-9A11-AFC06F06638A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20974DD2-EFB8-AF40-A79B-16AB13A48F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19600" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19600" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
     <sheet name="figure_order" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">figure_order!$A$1:$J$93</definedName>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="420">
   <si>
     <t>order</t>
   </si>
@@ -1094,9 +1093,6 @@
     <t>Outputs/Validation/revised/grobs/F6_S1_CP3182.rds</t>
   </si>
   <si>
-    <t>sf</t>
-  </si>
-  <si>
     <t>shrunk y and x axis</t>
   </si>
   <si>
@@ -1302,6 +1298,9 @@
   </si>
   <si>
     <t>ultimately failed this,a lot of noise and maybe something but quant peak just wasn’t organized enough. really nice co-eluting level 1 around 7.75 but not what algorithm picked</t>
+  </si>
+  <si>
+    <t>Outputs/Validation/revised/grobs/F6_S1_CP2475.rds</t>
   </si>
 </sst>
 </file>
@@ -1331,18 +1330,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1407,7 +1400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1426,7 +1419,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1434,10 +1427,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1786,7 +1775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E34" sqref="E34:E44"/>
     </sheetView>
@@ -2725,12 +2714,12 @@
       <c r="I30" s="2">
         <v>7.9249999999999998</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2759,12 +2748,12 @@
       <c r="I31" s="2">
         <v>4.45</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2793,12 +2782,12 @@
       <c r="I32" s="2">
         <v>4.45</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2827,12 +2816,12 @@
       <c r="I33" s="2">
         <v>16.574999999999999</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="J33" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2861,12 +2850,12 @@
       <c r="I34" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="J34" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2895,12 +2884,12 @@
       <c r="I35" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2929,12 +2918,12 @@
       <c r="I36" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J36" s="9" t="s">
+      <c r="J36" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2963,12 +2952,12 @@
       <c r="I37" s="2">
         <v>5.05</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,7 +2986,7 @@
       <c r="I38" s="2">
         <v>20.2</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K38" s="2"/>
@@ -3031,7 +3020,7 @@
       <c r="I39" s="2">
         <v>13.025</v>
       </c>
-      <c r="J39" s="9" t="s">
+      <c r="J39" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K39" s="2"/>
@@ -3065,7 +3054,7 @@
       <c r="I40" s="2">
         <v>5.2</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K40" s="2"/>
@@ -3099,7 +3088,7 @@
       <c r="I41" s="2">
         <v>6.25</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="J41" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K41" s="2"/>
@@ -3133,7 +3122,7 @@
       <c r="I42" s="2">
         <v>12.2</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="J42" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K42" s="2"/>
@@ -3167,7 +3156,7 @@
       <c r="I43" s="2">
         <v>6.6</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="J43" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K43" s="2"/>
@@ -3201,7 +3190,7 @@
       <c r="I44" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="J44" s="8" t="s">
         <v>323</v>
       </c>
       <c r="K44" s="2"/>
@@ -3237,11 +3226,11 @@
       <c r="I45" s="2">
         <v>7.55</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="J45" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L45" s="2"/>
     </row>
@@ -3273,11 +3262,11 @@
       <c r="I46" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J46" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>189</v>
@@ -3311,14 +3300,14 @@
       <c r="I47" s="2">
         <v>11.25</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -3349,11 +3338,11 @@
       <c r="I48" s="2">
         <v>17.45</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L48" s="2"/>
     </row>
@@ -3385,11 +3374,11 @@
       <c r="I49" s="2">
         <v>5.3</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="J49" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L49" s="2"/>
     </row>
@@ -3407,7 +3396,7 @@
         <v>222</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>223</v>
@@ -3421,11 +3410,11 @@
       <c r="I50" s="2">
         <v>12.875</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="J50" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L50" s="2"/>
     </row>
@@ -3457,11 +3446,11 @@
       <c r="I51" s="2">
         <v>7.4</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="J51" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L51" s="2"/>
     </row>
@@ -3493,11 +3482,11 @@
       <c r="I52" s="2">
         <v>6.45</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="J52" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L52" s="2"/>
     </row>
@@ -3529,11 +3518,11 @@
       <c r="I53" s="2">
         <v>6.25</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="J53" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L53" s="2"/>
     </row>
@@ -3565,11 +3554,11 @@
       <c r="I54" s="2">
         <v>6.55</v>
       </c>
-      <c r="J54" s="9" t="s">
+      <c r="J54" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>314</v>
@@ -3603,7 +3592,7 @@
       <c r="I55" s="2">
         <v>8.15</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="J55" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -3641,11 +3630,11 @@
       <c r="I56" s="2">
         <v>7.5250000000000004</v>
       </c>
-      <c r="J56" s="9" t="s">
+      <c r="J56" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>28</v>
@@ -3679,11 +3668,11 @@
       <c r="I57" s="2">
         <v>13.85</v>
       </c>
-      <c r="J57" s="9" t="s">
+      <c r="J57" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>276</v>
@@ -3717,11 +3706,11 @@
       <c r="I58" s="2">
         <v>13.45</v>
       </c>
-      <c r="J58" s="9" t="s">
+      <c r="J58" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>274</v>
@@ -3755,11 +3744,11 @@
       <c r="I59" s="2">
         <v>6.5</v>
       </c>
-      <c r="J59" s="9" t="s">
+      <c r="J59" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L59" s="2"/>
     </row>
@@ -3791,11 +3780,11 @@
       <c r="I60" s="2">
         <v>6.5</v>
       </c>
-      <c r="J60" s="9" t="s">
+      <c r="J60" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L60" s="2"/>
     </row>
@@ -3827,11 +3816,11 @@
       <c r="I61" s="2">
         <v>9.2249999999999996</v>
       </c>
-      <c r="J61" s="9" t="s">
+      <c r="J61" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L61" s="2"/>
     </row>
@@ -3863,11 +3852,11 @@
       <c r="I62" s="2">
         <v>9.7750000000000004</v>
       </c>
-      <c r="J62" s="9" t="s">
+      <c r="J62" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L62" s="2"/>
     </row>
@@ -3899,11 +3888,11 @@
       <c r="I63" s="2">
         <v>3.95</v>
       </c>
-      <c r="J63" s="9" t="s">
+      <c r="J63" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L63" s="2"/>
     </row>
@@ -3935,11 +3924,11 @@
       <c r="I64" s="2">
         <v>9.65</v>
       </c>
-      <c r="J64" s="9" t="s">
+      <c r="J64" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>296</v>
@@ -3973,11 +3962,11 @@
       <c r="I65" s="2">
         <v>11.3575</v>
       </c>
-      <c r="J65" s="9" t="s">
+      <c r="J65" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>252</v>
@@ -4011,11 +4000,11 @@
       <c r="I66" s="2">
         <v>22.45</v>
       </c>
-      <c r="J66" s="9" t="s">
+      <c r="J66" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L66" s="2"/>
     </row>
@@ -4047,11 +4036,11 @@
       <c r="I67" s="2">
         <v>9.65</v>
       </c>
-      <c r="J67" s="9" t="s">
+      <c r="J67" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>241</v>
@@ -4085,11 +4074,11 @@
       <c r="I68" s="2">
         <v>9.5500000000000007</v>
       </c>
-      <c r="J68" s="9" t="s">
+      <c r="J68" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>242</v>
@@ -4123,11 +4112,11 @@
       <c r="I69" s="2">
         <v>2.5</v>
       </c>
-      <c r="J69" s="9" t="s">
+      <c r="J69" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L69" s="2"/>
     </row>
@@ -4159,11 +4148,11 @@
       <c r="I70" s="2">
         <v>18.149999999999999</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="J70" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L70" s="2"/>
     </row>
@@ -4195,11 +4184,11 @@
       <c r="I71" s="2">
         <v>10.102499999999999</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="J71" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L71" s="2"/>
     </row>
@@ -4231,11 +4220,11 @@
       <c r="I72" s="2">
         <v>7.875</v>
       </c>
-      <c r="J72" s="9" t="s">
+      <c r="J72" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L72" s="2"/>
     </row>
@@ -4253,7 +4242,7 @@
         <v>164</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>165</v>
@@ -4267,11 +4256,11 @@
       <c r="I73" s="2">
         <v>6.75</v>
       </c>
-      <c r="J73" s="9" t="s">
+      <c r="J73" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L73" s="2"/>
     </row>
@@ -4303,11 +4292,11 @@
       <c r="I74" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J74" s="9" t="s">
+      <c r="J74" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L74" s="2"/>
     </row>
@@ -4339,7 +4328,7 @@
       <c r="I75" s="2">
         <v>10.1</v>
       </c>
-      <c r="J75" s="9" t="s">
+      <c r="J75" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K75" s="2" t="s">
@@ -4377,7 +4366,7 @@
       <c r="I76" s="2">
         <v>19.7</v>
       </c>
-      <c r="J76" s="9" t="s">
+      <c r="J76" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K76" s="2" t="s">
@@ -4415,7 +4404,7 @@
       <c r="I77" s="2">
         <v>18</v>
       </c>
-      <c r="J77" s="9" t="s">
+      <c r="J77" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K77" s="2" t="s">
@@ -4453,7 +4442,7 @@
       <c r="I78" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="J78" s="9" t="s">
+      <c r="J78" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K78" s="2" t="s">
@@ -4489,11 +4478,11 @@
       <c r="I79" s="2">
         <v>7.5</v>
       </c>
-      <c r="J79" s="9" t="s">
+      <c r="J79" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>244</v>
@@ -4527,7 +4516,7 @@
       <c r="I80" s="2">
         <v>3.9249999999999998</v>
       </c>
-      <c r="J80" s="9" t="s">
+      <c r="J80" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K80" s="2" t="s">
@@ -4565,7 +4554,7 @@
       <c r="I81" s="2">
         <v>8.35</v>
       </c>
-      <c r="J81" s="9" t="s">
+      <c r="J81" s="8" t="s">
         <v>320</v>
       </c>
       <c r="K81" s="2" t="s">
@@ -4586,10 +4575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4606,7 +4595,7 @@
     <col min="10" max="10" width="46.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4626,19 +4615,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>415</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4657,20 +4646,27 @@
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11">
-        <v>2</v>
-      </c>
-      <c r="H2" s="12">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>413</v>
+      <c r="G2" s="9">
+        <v>2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <f>_xlfn.XMATCH(L2,J:J)</f>
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4689,20 +4685,27 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11">
-        <v>2</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>416</v>
+      <c r="G3" s="9">
+        <v>2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="0">_xlfn.XMATCH(L3,J:J)</f>
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -4721,20 +4724,27 @@
       <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="11">
-        <v>2</v>
-      </c>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>413</v>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>15</v>
       </c>
@@ -4753,20 +4763,27 @@
       <c r="F5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="11">
-        <v>2</v>
-      </c>
-      <c r="H5" s="12">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>416</v>
+      <c r="G5" s="9">
+        <v>2</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>19</v>
       </c>
@@ -4785,20 +4802,27 @@
       <c r="F6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="11">
-        <v>2</v>
-      </c>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>413</v>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>19</v>
       </c>
@@ -4817,20 +4841,27 @@
       <c r="F7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="11">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>416</v>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>20</v>
       </c>
@@ -4849,20 +4880,27 @@
       <c r="F8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="11">
-        <v>2</v>
-      </c>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>413</v>
+      <c r="G8" s="9">
+        <v>2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>21</v>
       </c>
@@ -4881,20 +4919,27 @@
       <c r="F9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="11">
-        <v>2</v>
-      </c>
-      <c r="H9" s="12">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>416</v>
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>24</v>
       </c>
@@ -4913,20 +4958,27 @@
       <c r="F10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="11">
-        <v>2</v>
-      </c>
-      <c r="H10" s="12">
-        <v>1</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>413</v>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>24</v>
       </c>
@@ -4945,20 +4997,27 @@
       <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="11">
-        <v>2</v>
-      </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>416</v>
+      <c r="G11" s="9">
+        <v>2</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>26</v>
       </c>
@@ -4977,20 +5036,27 @@
       <c r="F12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="11">
-        <v>2</v>
-      </c>
-      <c r="H12" s="12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>413</v>
+      <c r="G12" s="9">
+        <v>2</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>27</v>
       </c>
@@ -5009,20 +5075,27 @@
       <c r="F13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="11">
-        <v>2</v>
-      </c>
-      <c r="H13" s="12">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>416</v>
+      <c r="G13" s="9">
+        <v>2</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>29</v>
       </c>
@@ -5041,20 +5114,27 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="11">
-        <v>2</v>
-      </c>
-      <c r="H14" s="12">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>413</v>
+      <c r="G14" s="9">
+        <v>2</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>29.5</v>
       </c>
@@ -5068,25 +5148,32 @@
         <v>333</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G15" s="9">
+        <v>2</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="G15" s="11">
-        <v>2</v>
-      </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L15" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>30</v>
       </c>
@@ -5105,20 +5192,27 @@
       <c r="F16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="11">
-        <v>2</v>
-      </c>
-      <c r="H16" s="12">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>413</v>
+      <c r="G16" s="9">
+        <v>2</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="L16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>30</v>
       </c>
@@ -5137,20 +5231,27 @@
       <c r="F17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="11">
-        <v>2</v>
-      </c>
-      <c r="H17" s="12">
-        <v>1</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>416</v>
+      <c r="G17" s="9">
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="L17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>34</v>
       </c>
@@ -5169,21 +5270,28 @@
       <c r="F18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="11">
-        <v>2</v>
-      </c>
-      <c r="H18" s="12">
-        <v>1</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>413</v>
+      <c r="G18" s="9">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+        <v>387</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
         <v>34.5</v>
       </c>
       <c r="B19" s="3">
@@ -5199,22 +5307,29 @@
         <v>103</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G19" s="11">
-        <v>2</v>
-      </c>
-      <c r="H19" s="12">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>35</v>
       </c>
@@ -5233,20 +5348,27 @@
       <c r="F20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="11">
-        <v>2</v>
-      </c>
-      <c r="H20" s="12">
-        <v>1</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>413</v>
+      <c r="G20" s="9">
+        <v>2</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="L20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>35</v>
       </c>
@@ -5265,20 +5387,27 @@
       <c r="F21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="11">
-        <v>2</v>
-      </c>
-      <c r="H21" s="12">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>416</v>
+      <c r="G21" s="9">
+        <v>2</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="L21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>36</v>
       </c>
@@ -5297,20 +5426,27 @@
       <c r="F22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="11">
-        <v>2</v>
-      </c>
-      <c r="H22" s="12">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>413</v>
+      <c r="G22" s="9">
+        <v>2</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="L22" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>36.5</v>
       </c>
@@ -5327,22 +5463,29 @@
         <v>109</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G23" s="11">
-        <v>2</v>
-      </c>
-      <c r="H23" s="12">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="L23" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42</v>
       </c>
@@ -5361,20 +5504,27 @@
       <c r="F24" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="11">
-        <v>2</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>413</v>
+      <c r="G24" s="9">
+        <v>2</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="L24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42</v>
       </c>
@@ -5393,20 +5543,27 @@
       <c r="F25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="11">
-        <v>2</v>
-      </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>416</v>
+      <c r="G25" s="9">
+        <v>2</v>
+      </c>
+      <c r="H25" s="10">
+        <v>1</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="L25" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43</v>
       </c>
@@ -5425,20 +5582,27 @@
       <c r="F26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="11">
-        <v>2</v>
-      </c>
-      <c r="H26" s="12">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>413</v>
+      <c r="G26" s="9">
+        <v>2</v>
+      </c>
+      <c r="H26" s="10">
+        <v>1</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="L26" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43.5</v>
       </c>
@@ -5452,25 +5616,32 @@
         <v>333</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G27" s="9">
+        <v>2</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="G27" s="11">
-        <v>2</v>
-      </c>
-      <c r="H27" s="12">
-        <v>1</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="L27" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>47</v>
       </c>
@@ -5489,20 +5660,27 @@
       <c r="F28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="11">
-        <v>2</v>
-      </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>413</v>
+      <c r="G28" s="9">
+        <v>2</v>
+      </c>
+      <c r="H28" s="10">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>47</v>
       </c>
@@ -5521,20 +5699,27 @@
       <c r="F29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G29" s="11">
-        <v>2</v>
-      </c>
-      <c r="H29" s="12">
-        <v>1</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>416</v>
+      <c r="G29" s="9">
+        <v>2</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>48</v>
       </c>
@@ -5553,20 +5738,27 @@
       <c r="F30" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G30" s="11">
-        <v>2</v>
-      </c>
-      <c r="H30" s="12">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>413</v>
+      <c r="G30" s="9">
+        <v>2</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="L30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>48.5</v>
       </c>
@@ -5580,25 +5772,32 @@
         <v>333</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G31" s="9">
+        <v>2</v>
+      </c>
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="G31" s="11">
-        <v>2</v>
-      </c>
-      <c r="H31" s="12">
-        <v>1</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="L31" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>49</v>
       </c>
@@ -5617,20 +5816,27 @@
       <c r="F32" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G32" s="11">
-        <v>2</v>
-      </c>
-      <c r="H32" s="12">
-        <v>1</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>413</v>
+      <c r="G32" s="9">
+        <v>2</v>
+      </c>
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>49</v>
       </c>
@@ -5649,20 +5855,27 @@
       <c r="F33" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="11">
-        <v>2</v>
-      </c>
-      <c r="H33" s="12">
-        <v>1</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>416</v>
+      <c r="G33" s="9">
+        <v>2</v>
+      </c>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>54</v>
       </c>
@@ -5681,20 +5894,27 @@
       <c r="F34" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G34" s="11">
-        <v>2</v>
-      </c>
-      <c r="H34" s="12">
-        <v>1</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>413</v>
+      <c r="G34" s="9">
+        <v>2</v>
+      </c>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="L34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>54</v>
       </c>
@@ -5713,20 +5933,27 @@
       <c r="F35" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G35" s="11">
-        <v>2</v>
-      </c>
-      <c r="H35" s="12">
-        <v>1</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>416</v>
+      <c r="G35" s="9">
+        <v>2</v>
+      </c>
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L35" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>55</v>
       </c>
@@ -5745,20 +5972,27 @@
       <c r="F36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G36" s="11">
-        <v>2</v>
-      </c>
-      <c r="H36" s="12">
-        <v>1</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>413</v>
+      <c r="G36" s="9">
+        <v>2</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="L36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>55.5</v>
       </c>
@@ -5772,25 +6006,32 @@
         <v>333</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G37" s="9">
+        <v>2</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="G37" s="11">
-        <v>2</v>
-      </c>
-      <c r="H37" s="12">
-        <v>1</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="L37" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>56</v>
       </c>
@@ -5809,20 +6050,27 @@
       <c r="F38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="11">
-        <v>2</v>
-      </c>
-      <c r="H38" s="12">
-        <v>1</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>413</v>
+      <c r="G38" s="9">
+        <v>2</v>
+      </c>
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L38" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>56</v>
       </c>
@@ -5841,20 +6089,27 @@
       <c r="F39" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G39" s="11">
-        <v>2</v>
-      </c>
-      <c r="H39" s="12">
-        <v>1</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>416</v>
+      <c r="G39" s="9">
+        <v>2</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="L39" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>59</v>
       </c>
@@ -5873,20 +6128,27 @@
       <c r="F40" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G40" s="11">
-        <v>2</v>
-      </c>
-      <c r="H40" s="12">
-        <v>1</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>413</v>
+      <c r="G40" s="9">
+        <v>2</v>
+      </c>
+      <c r="H40" s="10">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="L40" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>59</v>
       </c>
@@ -5905,20 +6167,27 @@
       <c r="F41" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G41" s="11">
-        <v>2</v>
-      </c>
-      <c r="H41" s="12">
-        <v>1</v>
-      </c>
-      <c r="I41" s="15" t="s">
-        <v>416</v>
+      <c r="G41" s="9">
+        <v>2</v>
+      </c>
+      <c r="H41" s="10">
+        <v>1</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="L41" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>60</v>
       </c>
@@ -5937,20 +6206,27 @@
       <c r="F42" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="11">
-        <v>2</v>
-      </c>
-      <c r="H42" s="12">
-        <v>1</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>413</v>
+      <c r="G42" s="9">
+        <v>2</v>
+      </c>
+      <c r="H42" s="10">
+        <v>1</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L42" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>62</v>
       </c>
@@ -5969,20 +6245,27 @@
       <c r="F43" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G43" s="11">
-        <v>2</v>
-      </c>
-      <c r="H43" s="12">
-        <v>1</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>416</v>
+      <c r="G43" s="9">
+        <v>2</v>
+      </c>
+      <c r="H43" s="10">
+        <v>1</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="L43" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>5</v>
       </c>
@@ -6001,20 +6284,27 @@
       <c r="F44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G44" s="13">
-        <v>2</v>
-      </c>
-      <c r="H44" s="14">
-        <v>2</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>413</v>
+      <c r="G44" s="11">
+        <v>2</v>
+      </c>
+      <c r="H44" s="12">
+        <v>2</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L44" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>8</v>
       </c>
@@ -6033,20 +6323,27 @@
       <c r="F45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G45" s="13">
-        <v>2</v>
-      </c>
-      <c r="H45" s="14">
-        <v>2</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>416</v>
+      <c r="G45" s="11">
+        <v>2</v>
+      </c>
+      <c r="H45" s="12">
+        <v>2</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+      <c r="K45" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L45" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>33</v>
       </c>
@@ -6065,20 +6362,27 @@
       <c r="F46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="13">
-        <v>2</v>
-      </c>
-      <c r="H46" s="14">
-        <v>2</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>413</v>
+      <c r="G46" s="11">
+        <v>2</v>
+      </c>
+      <c r="H46" s="12">
+        <v>2</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="L46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>39</v>
       </c>
@@ -6097,20 +6401,27 @@
       <c r="F47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G47" s="13">
-        <v>2</v>
-      </c>
-      <c r="H47" s="14">
-        <v>2</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>416</v>
+      <c r="G47" s="11">
+        <v>2</v>
+      </c>
+      <c r="H47" s="12">
+        <v>2</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L47" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>51</v>
       </c>
@@ -6129,20 +6440,27 @@
       <c r="F48" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="13">
-        <v>2</v>
-      </c>
-      <c r="H48" s="14">
-        <v>2</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>413</v>
+      <c r="G48" s="11">
+        <v>2</v>
+      </c>
+      <c r="H48" s="12">
+        <v>2</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="L48" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>51</v>
       </c>
@@ -6161,20 +6479,27 @@
       <c r="F49" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G49" s="13">
-        <v>2</v>
-      </c>
-      <c r="H49" s="14">
-        <v>2</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>416</v>
+      <c r="G49" s="11">
+        <v>2</v>
+      </c>
+      <c r="H49" s="12">
+        <v>2</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L49" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -6193,20 +6518,27 @@
       <c r="F50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="9">
         <v>3</v>
       </c>
-      <c r="H50" s="12">
-        <v>1</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>413</v>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="L50" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>1</v>
       </c>
@@ -6225,20 +6557,27 @@
       <c r="F51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="9">
         <v>3</v>
       </c>
-      <c r="H51" s="12">
-        <v>1</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>416</v>
+      <c r="H51" s="10">
+        <v>1</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="L51" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>64</v>
       </c>
@@ -6257,20 +6596,27 @@
       <c r="F52" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="9">
         <v>3</v>
       </c>
-      <c r="H52" s="12">
-        <v>1</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>413</v>
+      <c r="H52" s="10">
+        <v>1</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="L52" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>65</v>
       </c>
@@ -6289,20 +6635,24 @@
       <c r="F53" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="9">
         <v>3</v>
       </c>
-      <c r="H53" s="12">
-        <v>1</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>416</v>
+      <c r="H53" s="10">
+        <v>1</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>72</v>
       </c>
@@ -6321,20 +6671,24 @@
       <c r="F54" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G54" s="9">
         <v>3</v>
       </c>
-      <c r="H54" s="12">
-        <v>1</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>413</v>
+      <c r="H54" s="10">
+        <v>1</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>72</v>
       </c>
@@ -6351,22 +6705,26 @@
         <v>214</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="G55" s="9">
+        <v>3</v>
+      </c>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G55" s="11">
-        <v>3</v>
-      </c>
-      <c r="H55" s="12">
-        <v>1</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>71</v>
       </c>
@@ -6385,20 +6743,24 @@
       <c r="F56" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="11">
         <v>3</v>
       </c>
-      <c r="H56" s="14">
-        <v>2</v>
-      </c>
-      <c r="I56" s="9" t="s">
-        <v>413</v>
+      <c r="H56" s="12">
+        <v>2</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>74</v>
       </c>
@@ -6417,20 +6779,24 @@
       <c r="F57" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="11">
         <v>3</v>
       </c>
-      <c r="H57" s="14">
-        <v>2</v>
-      </c>
-      <c r="I57" s="15" t="s">
-        <v>416</v>
+      <c r="H57" s="12">
+        <v>2</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>75</v>
       </c>
@@ -6449,20 +6815,24 @@
       <c r="F58" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="11">
         <v>3</v>
       </c>
-      <c r="H58" s="14">
-        <v>2</v>
-      </c>
-      <c r="I58" s="9" t="s">
-        <v>413</v>
+      <c r="H58" s="12">
+        <v>2</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>77</v>
       </c>
@@ -6481,111 +6851,239 @@
       <c r="F59" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="11">
         <v>3</v>
       </c>
-      <c r="H59" s="14">
-        <v>2</v>
-      </c>
-      <c r="I59" s="15" t="s">
-        <v>416</v>
+      <c r="H59" s="12">
+        <v>2</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>415</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C60"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C61"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C63"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C64"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C65"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C66"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C67"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <f t="shared" ref="K67:K90" si="1">_xlfn.XMATCH(L67,J:J)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C68"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C69"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C70"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C71"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C72"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C73"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C74"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C75"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C76"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C77"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C78"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K78">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C79"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C80"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C81"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K81">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C82"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C83"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C84"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C85"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C86"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C87"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C88"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C89"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C90"/>
+      <c r="K90">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J93" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
@@ -6599,69 +7097,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE26EEA-4CF4-724E-BE9F-DA01257F77DB}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="8">
-        <v>2</v>
-      </c>
-      <c r="H2" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed title names for fragments
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20974DD2-EFB8-AF40-A79B-16AB13A48F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31223C6D-5563-ED4C-B580-8FCAF8991FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19600" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="419">
   <si>
     <t>order</t>
   </si>
@@ -1298,9 +1298,6 @@
   </si>
   <si>
     <t>ultimately failed this,a lot of noise and maybe something but quant peak just wasn’t organized enough. really nice co-eluting level 1 around 7.75 but not what algorithm picked</t>
-  </si>
-  <si>
-    <t>Outputs/Validation/revised/grobs/F6_S1_CP2475.rds</t>
   </si>
 </sst>
 </file>
@@ -4575,10 +4572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="K37" sqref="K1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4595,7 +4592,7 @@
     <col min="10" max="10" width="46.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4627,7 +4624,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4658,15 +4655,8 @@
       <c r="J2" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="K2">
-        <f>_xlfn.XMATCH(L2,J:J)</f>
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4697,15 +4687,8 @@
       <c r="J3" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K66" si="0">_xlfn.XMATCH(L3,J:J)</f>
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -4736,15 +4719,8 @@
       <c r="J4" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>15</v>
       </c>
@@ -4775,15 +4751,8 @@
       <c r="J5" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>19</v>
       </c>
@@ -4814,15 +4783,8 @@
       <c r="J6" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L6" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>19</v>
       </c>
@@ -4853,15 +4815,8 @@
       <c r="J7" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L7" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>20</v>
       </c>
@@ -4892,15 +4847,8 @@
       <c r="J8" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="L8" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>21</v>
       </c>
@@ -4931,15 +4879,8 @@
       <c r="J9" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="L9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>24</v>
       </c>
@@ -4970,15 +4911,8 @@
       <c r="J10" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>24</v>
       </c>
@@ -5009,15 +4943,8 @@
       <c r="J11" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="L11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>26</v>
       </c>
@@ -5048,15 +4975,8 @@
       <c r="J12" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L12" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>27</v>
       </c>
@@ -5087,15 +5007,8 @@
       <c r="J13" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L13" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>29</v>
       </c>
@@ -5126,15 +5039,8 @@
       <c r="J14" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="L14" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>29.5</v>
       </c>
@@ -5165,15 +5071,8 @@
       <c r="J15" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="L15" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>30</v>
       </c>
@@ -5204,15 +5103,8 @@
       <c r="J16" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="L16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>30</v>
       </c>
@@ -5243,15 +5135,8 @@
       <c r="J17" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="L17" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>34</v>
       </c>
@@ -5282,15 +5167,8 @@
       <c r="J18" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="L18" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>34.5</v>
       </c>
@@ -5321,15 +5199,8 @@
       <c r="J19" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L19" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>35</v>
       </c>
@@ -5360,15 +5231,8 @@
       <c r="J20" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="L20" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>35</v>
       </c>
@@ -5399,15 +5263,8 @@
       <c r="J21" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="L21" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>36</v>
       </c>
@@ -5438,15 +5295,8 @@
       <c r="J22" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="L22" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>36.5</v>
       </c>
@@ -5477,15 +5327,8 @@
       <c r="J23" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="L23" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42</v>
       </c>
@@ -5516,15 +5359,8 @@
       <c r="J24" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="L24" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42</v>
       </c>
@@ -5555,15 +5391,8 @@
       <c r="J25" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="L25" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43</v>
       </c>
@@ -5594,15 +5423,8 @@
       <c r="J26" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="L26" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43.5</v>
       </c>
@@ -5633,15 +5455,8 @@
       <c r="J27" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="L27" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>47</v>
       </c>
@@ -5672,15 +5487,8 @@
       <c r="J28" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L28" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>47</v>
       </c>
@@ -5711,15 +5519,8 @@
       <c r="J29" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L29" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>48</v>
       </c>
@@ -5750,15 +5551,8 @@
       <c r="J30" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L30" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>48.5</v>
       </c>
@@ -5789,15 +5583,8 @@
       <c r="J31" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="L31" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>49</v>
       </c>
@@ -5828,15 +5615,8 @@
       <c r="J32" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L32" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>49</v>
       </c>
@@ -5867,15 +5647,8 @@
       <c r="J33" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L33" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>54</v>
       </c>
@@ -5906,15 +5679,8 @@
       <c r="J34" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="L34" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>54</v>
       </c>
@@ -5945,15 +5711,8 @@
       <c r="J35" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L35" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>55</v>
       </c>
@@ -5984,15 +5743,8 @@
       <c r="J36" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="L36" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>55.5</v>
       </c>
@@ -6023,15 +5775,8 @@
       <c r="J37" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="L37" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>56</v>
       </c>
@@ -6062,15 +5807,8 @@
       <c r="J38" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L38" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>56</v>
       </c>
@@ -6101,15 +5839,8 @@
       <c r="J39" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="L39" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>59</v>
       </c>
@@ -6140,15 +5871,8 @@
       <c r="J40" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="L40" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>59</v>
       </c>
@@ -6179,15 +5903,8 @@
       <c r="J41" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="L41" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>60</v>
       </c>
@@ -6218,15 +5935,8 @@
       <c r="J42" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="K42">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="L42" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>62</v>
       </c>
@@ -6257,15 +5967,8 @@
       <c r="J43" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="L43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>5</v>
       </c>
@@ -6296,15 +5999,8 @@
       <c r="J44" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="K44">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="L44" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>8</v>
       </c>
@@ -6335,15 +6031,8 @@
       <c r="J45" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K45" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L45" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>33</v>
       </c>
@@ -6374,15 +6063,8 @@
       <c r="J46" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="K46">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L46" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>39</v>
       </c>
@@ -6413,15 +6095,8 @@
       <c r="J47" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="K47">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L47" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>51</v>
       </c>
@@ -6452,15 +6127,8 @@
       <c r="J48" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="L48" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>51</v>
       </c>
@@ -6491,15 +6159,8 @@
       <c r="J49" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L49" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -6530,15 +6191,8 @@
       <c r="J50" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="K50">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="L50" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>1</v>
       </c>
@@ -6569,15 +6223,8 @@
       <c r="J51" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="K51">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="L51" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>64</v>
       </c>
@@ -6608,15 +6255,8 @@
       <c r="J52" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="L52" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>65</v>
       </c>
@@ -6647,12 +6287,8 @@
       <c r="J53" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="K53">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>72</v>
       </c>
@@ -6683,12 +6319,8 @@
       <c r="J54" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="K54">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>72</v>
       </c>
@@ -6719,12 +6351,8 @@
       <c r="J55" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K55">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>71</v>
       </c>
@@ -6755,12 +6383,8 @@
       <c r="J56" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="K56">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>74</v>
       </c>
@@ -6791,12 +6415,8 @@
       <c r="J57" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="K57">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>75</v>
       </c>
@@ -6827,12 +6447,8 @@
       <c r="J58" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="K58">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>77</v>
       </c>
@@ -6863,227 +6479,99 @@
       <c r="J59" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="K59">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C60"/>
-      <c r="K60">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C61"/>
-      <c r="K61">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C62"/>
-      <c r="K62">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C63"/>
-      <c r="K63">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C64"/>
-      <c r="K64">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65"/>
-      <c r="K65">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66"/>
-      <c r="K66">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67"/>
-      <c r="K67">
-        <f t="shared" ref="K67:K90" si="1">_xlfn.XMATCH(L67,J:J)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68"/>
-      <c r="K68">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69"/>
-      <c r="K69">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70"/>
-      <c r="K70">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71"/>
-      <c r="K71">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72"/>
-      <c r="K72">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73"/>
-      <c r="K73">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74"/>
-      <c r="K74">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75"/>
-      <c r="K75">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76"/>
-      <c r="K76">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77"/>
-      <c r="K77">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78"/>
-      <c r="K78">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79"/>
-      <c r="K79">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80"/>
-      <c r="K80">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81"/>
-      <c r="K81">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82"/>
-      <c r="K82">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83"/>
-      <c r="K83">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84"/>
-      <c r="K84">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="85" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85"/>
-      <c r="K85">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="86" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86"/>
-      <c r="K86">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87"/>
-      <c r="K87">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88"/>
-      <c r="K88">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="89" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89"/>
-      <c r="K89">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="90" spans="3:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90"/>
-      <c r="K90">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J93" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">

</xml_diff>

<commit_message>
finshed SF2 and SF3
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31223C6D-5563-ED4C-B580-8FCAF8991FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E14E4-CDE4-B94E-9507-41856528B21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19600" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19580" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
     <sheet name="figure_order" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">figure_order!$A$1:$J$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">figure_order!$A$1:$J$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">validation!$A$1:$L$81</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="420">
   <si>
     <t>order</t>
   </si>
@@ -1162,9 +1162,6 @@
     <t>zoomed x and y, not great but coelution in both so bumped to level 1</t>
   </si>
   <si>
-    <t>likely a matrix effect as the standard coelutes to far right</t>
-  </si>
-  <si>
     <t>F3_S1_CP3013</t>
   </si>
   <si>
@@ -1298,6 +1295,12 @@
   </si>
   <si>
     <t>ultimately failed this,a lot of noise and maybe something but quant peak just wasn’t organized enough. really nice co-eluting level 1 around 7.75 but not what algorithm picked</t>
+  </si>
+  <si>
+    <t>likely a matrix effect as the standard coelutes to far right… actually going to change back to 1</t>
+  </si>
+  <si>
+    <t>gamma-BHC</t>
   </si>
 </sst>
 </file>
@@ -1772,9 +1775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34:E44"/>
+    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2716,7 +2719,7 @@
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2750,7 +2753,7 @@
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -3289,7 +3292,7 @@
         <v>120</v>
       </c>
       <c r="G47" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" s="2">
         <v>11.05</v>
@@ -3304,7 +3307,7 @@
         <v>370</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>373</v>
+        <v>418</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -3393,7 +3396,7 @@
         <v>222</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>223</v>
@@ -4239,7 +4242,7 @@
         <v>164</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>165</v>
@@ -4572,10 +4575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="K37" sqref="K1:N1048576"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4612,13 +4615,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>414</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>267</v>
@@ -4650,7 +4653,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>343</v>
@@ -4682,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>342</v>
@@ -4714,10 +4717,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -4746,10 +4749,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -4778,7 +4781,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>341</v>
@@ -4810,7 +4813,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>340</v>
@@ -4842,10 +4845,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -4874,10 +4877,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -4906,10 +4909,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -4938,10 +4941,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -4970,10 +4973,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -5002,10 +5005,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -5034,10 +5037,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -5054,22 +5057,22 @@
         <v>333</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G15" s="9">
+        <v>2</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="G15" s="9">
-        <v>2</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -5098,10 +5101,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -5130,10 +5133,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -5162,10 +5165,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -5185,19 +5188,19 @@
         <v>103</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="G19" s="9">
-        <v>2</v>
-      </c>
-      <c r="H19" s="10">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -5226,10 +5229,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -5258,10 +5261,10 @@
         <v>1</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -5290,10 +5293,10 @@
         <v>1</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -5313,24 +5316,24 @@
         <v>109</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="G23" s="9">
-        <v>2</v>
-      </c>
-      <c r="H23" s="10">
-        <v>1</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -5342,10 +5345,10 @@
         <v>333</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G24" s="9">
         <v>2</v>
@@ -5354,15 +5357,15 @@
         <v>1</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>338</v>
+        <v>398</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>42</v>
+        <v>39.5</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -5374,10 +5377,10 @@
         <v>333</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>127</v>
+        <v>415</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>415</v>
       </c>
       <c r="G25" s="9">
         <v>2</v>
@@ -5386,15 +5389,15 @@
         <v>1</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>337</v>
+        <v>416</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -5406,10 +5409,10 @@
         <v>333</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G26" s="9">
         <v>2</v>
@@ -5418,15 +5421,15 @@
         <v>1</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>43.5</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -5438,10 +5441,10 @@
         <v>333</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>416</v>
+        <v>127</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>416</v>
+        <v>128</v>
       </c>
       <c r="G27" s="9">
         <v>2</v>
@@ -5450,15 +5453,15 @@
         <v>1</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>417</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -5470,10 +5473,10 @@
         <v>333</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G28" s="9">
         <v>2</v>
@@ -5482,15 +5485,15 @@
         <v>1</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>47</v>
+        <v>43.5</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -5502,10 +5505,10 @@
         <v>333</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>140</v>
+        <v>415</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>141</v>
+        <v>415</v>
       </c>
       <c r="G29" s="9">
         <v>2</v>
@@ -5514,15 +5517,15 @@
         <v>1</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -5534,10 +5537,10 @@
         <v>333</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G30" s="9">
         <v>2</v>
@@ -5546,15 +5549,15 @@
         <v>1</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>48.5</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -5566,10 +5569,10 @@
         <v>333</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>416</v>
+        <v>140</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>416</v>
+        <v>141</v>
       </c>
       <c r="G31" s="9">
         <v>2</v>
@@ -5578,15 +5581,15 @@
         <v>1</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
@@ -5598,10 +5601,10 @@
         <v>333</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="G32" s="9">
         <v>2</v>
@@ -5610,15 +5613,15 @@
         <v>1</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>336</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>49</v>
+        <v>48.5</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -5630,10 +5633,10 @@
         <v>333</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>147</v>
+        <v>415</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>415</v>
       </c>
       <c r="G33" s="9">
         <v>2</v>
@@ -5642,15 +5645,15 @@
         <v>1</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>335</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
@@ -5662,10 +5665,10 @@
         <v>333</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="G34" s="9">
         <v>2</v>
@@ -5674,15 +5677,15 @@
         <v>1</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>402</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
@@ -5694,10 +5697,10 @@
         <v>333</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="G35" s="9">
         <v>2</v>
@@ -5706,15 +5709,15 @@
         <v>1</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>401</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -5726,10 +5729,10 @@
         <v>333</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G36" s="9">
         <v>2</v>
@@ -5738,15 +5741,15 @@
         <v>1</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>55.5</v>
+        <v>54</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -5758,10 +5761,10 @@
         <v>333</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>416</v>
+        <v>161</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>416</v>
+        <v>162</v>
       </c>
       <c r="G37" s="9">
         <v>2</v>
@@ -5770,15 +5773,15 @@
         <v>1</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
@@ -5790,10 +5793,10 @@
         <v>333</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G38" s="9">
         <v>2</v>
@@ -5802,15 +5805,15 @@
         <v>1</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>56</v>
+        <v>55.5</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
@@ -5822,10 +5825,10 @@
         <v>333</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>166</v>
+        <v>415</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>167</v>
+        <v>415</v>
       </c>
       <c r="G39" s="9">
         <v>2</v>
@@ -5834,15 +5837,15 @@
         <v>1</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>348</v>
+        <v>416</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
@@ -5854,10 +5857,10 @@
         <v>333</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G40" s="9">
         <v>2</v>
@@ -5866,15 +5869,15 @@
         <v>1</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
@@ -5886,10 +5889,10 @@
         <v>333</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G41" s="9">
         <v>2</v>
@@ -5898,15 +5901,15 @@
         <v>1</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="3">
         <v>1</v>
@@ -5918,10 +5921,10 @@
         <v>333</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G42" s="9">
         <v>2</v>
@@ -5930,15 +5933,15 @@
         <v>1</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -5950,10 +5953,10 @@
         <v>333</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G43" s="9">
         <v>2</v>
@@ -5962,18 +5965,18 @@
         <v>1</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="B44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>334</v>
@@ -5982,30 +5985,30 @@
         <v>333</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>16</v>
+        <v>177</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" s="11">
-        <v>2</v>
-      </c>
-      <c r="H44" s="12">
-        <v>2</v>
+        <v>178</v>
+      </c>
+      <c r="G44" s="9">
+        <v>2</v>
+      </c>
+      <c r="H44" s="10">
+        <v>1</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>339</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>334</v>
@@ -6014,27 +6017,27 @@
         <v>333</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G45" s="11">
-        <v>2</v>
-      </c>
-      <c r="H45" s="12">
-        <v>2</v>
+        <v>184</v>
+      </c>
+      <c r="G45" s="9">
+        <v>2</v>
+      </c>
+      <c r="H45" s="10">
+        <v>1</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B46" s="3">
         <v>2</v>
@@ -6046,10 +6049,10 @@
         <v>333</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="G46" s="11">
         <v>2</v>
@@ -6058,15 +6061,15 @@
         <v>2</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
@@ -6078,10 +6081,10 @@
         <v>333</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>119</v>
+        <v>26</v>
       </c>
       <c r="G47" s="11">
         <v>2</v>
@@ -6090,15 +6093,15 @@
         <v>2</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B48" s="3">
         <v>2</v>
@@ -6110,10 +6113,10 @@
         <v>333</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="G48" s="11">
         <v>2</v>
@@ -6122,15 +6125,15 @@
         <v>2</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B49" s="3">
         <v>2</v>
@@ -6142,10 +6145,10 @@
         <v>333</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>152</v>
+        <v>415</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>153</v>
+        <v>415</v>
       </c>
       <c r="G49" s="11">
         <v>2</v>
@@ -6154,79 +6157,79 @@
         <v>2</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>344</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>333</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="9">
-        <v>3</v>
-      </c>
-      <c r="H50" s="10">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="G50" s="11">
+        <v>2</v>
+      </c>
+      <c r="H50" s="12">
+        <v>2</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>333</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="9">
-        <v>3</v>
-      </c>
-      <c r="H51" s="10">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="G51" s="11">
+        <v>2</v>
+      </c>
+      <c r="H51" s="12">
+        <v>2</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -6235,13 +6238,13 @@
         <v>333</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>196</v>
+        <v>4</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>197</v>
+        <v>5</v>
       </c>
       <c r="G52" s="9">
         <v>3</v>
@@ -6250,15 +6253,15 @@
         <v>1</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
@@ -6267,13 +6270,13 @@
         <v>333</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>199</v>
+        <v>4</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>235</v>
+        <v>5</v>
       </c>
       <c r="G53" s="9">
         <v>3</v>
@@ -6282,15 +6285,15 @@
         <v>1</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>378</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
@@ -6302,10 +6305,10 @@
         <v>334</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="G54" s="9">
         <v>3</v>
@@ -6314,15 +6317,15 @@
         <v>1</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
@@ -6334,10 +6337,10 @@
         <v>334</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="G55" s="9">
         <v>3</v>
@@ -6346,18 +6349,18 @@
         <v>1</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>333</v>
@@ -6366,30 +6369,30 @@
         <v>334</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G56" s="11">
+        <v>215</v>
+      </c>
+      <c r="G56" s="9">
         <v>3</v>
       </c>
-      <c r="H56" s="12">
-        <v>2</v>
+      <c r="H56" s="10">
+        <v>1</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>333</v>
@@ -6398,27 +6401,27 @@
         <v>334</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G57" s="11">
+        <v>415</v>
+      </c>
+      <c r="G57" s="9">
         <v>3</v>
       </c>
-      <c r="H57" s="12">
-        <v>2</v>
+      <c r="H57" s="10">
+        <v>1</v>
       </c>
       <c r="I57" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>383</v>
+        <v>416</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B58" s="3">
         <v>2</v>
@@ -6430,10 +6433,10 @@
         <v>334</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G58" s="11">
         <v>3</v>
@@ -6442,15 +6445,15 @@
         <v>2</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B59" s="3">
         <v>2</v>
@@ -6462,10 +6465,10 @@
         <v>334</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="G59" s="11">
         <v>3</v>
@@ -6474,17 +6477,75 @@
         <v>2</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C60"/>
+      <c r="A60" s="2">
+        <v>75</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G60" s="11">
+        <v>3</v>
+      </c>
+      <c r="H60" s="12">
+        <v>2</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C61"/>
+      <c r="A61" s="2">
+        <v>77</v>
+      </c>
+      <c r="B61" s="3">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G61" s="11">
+        <v>3</v>
+      </c>
+      <c r="H61" s="12">
+        <v>2</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C62"/>
@@ -6573,13 +6634,19 @@
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90"/>
     </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J93" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J93">
-      <sortCondition ref="G1:G93"/>
+  <autoFilter ref="A1:J95" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J95">
+      <sortCondition ref="G1:G95"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="F1:F19 F21:F32 F34:F1048576">
+  <conditionalFormatting sqref="F1:F19 F21:F33 F35:F1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
done working for 12/16
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E14E4-CDE4-B94E-9507-41856528B21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D70187-624A-3643-98F0-FBB4173DFF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19580" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19580" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -1775,9 +1775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4577,8 +4577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated rtx fxn to tag cadaver files with C_
</commit_message>
<xml_diff>
--- a/metadata_files/validation.xlsx
+++ b/metadata_files/validation.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D70187-624A-3643-98F0-FBB4173DFF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5714548F-708C-E246-A69E-B1D1ABB28ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19580" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38020" windowHeight="19580" activeTab="1" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
-    <sheet name="figure_order" sheetId="2" r:id="rId2"/>
+    <sheet name="validation_cadaver" sheetId="3" r:id="rId2"/>
+    <sheet name="figure_order" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">figure_order!$A$1:$J$95</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">validation!$A$1:$L$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">figure_order!$A$1:$J$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">validation!$A$1:$M$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">validation_cadaver!$A$1:$M$9</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="493">
   <si>
     <t>order</t>
   </si>
@@ -1301,6 +1303,225 @@
   </si>
   <si>
     <t>gamma-BHC</t>
+  </si>
+  <si>
+    <t>cas</t>
+  </si>
+  <si>
+    <t>87-86-5</t>
+  </si>
+  <si>
+    <t>58-89-9</t>
+  </si>
+  <si>
+    <t>72-43-5</t>
+  </si>
+  <si>
+    <t>2642-71-9</t>
+  </si>
+  <si>
+    <t>72-56-0</t>
+  </si>
+  <si>
+    <t>30667-99-3</t>
+  </si>
+  <si>
+    <t>85-40-5</t>
+  </si>
+  <si>
+    <t>1912-24-9</t>
+  </si>
+  <si>
+    <t>41483-43-6</t>
+  </si>
+  <si>
+    <t>5915-41-3</t>
+  </si>
+  <si>
+    <t>57837-19-1</t>
+  </si>
+  <si>
+    <t>84-74-2</t>
+  </si>
+  <si>
+    <t>117-84-0</t>
+  </si>
+  <si>
+    <t>621-64-7</t>
+  </si>
+  <si>
+    <t>95-48-7</t>
+  </si>
+  <si>
+    <t>88-74-4</t>
+  </si>
+  <si>
+    <t>92-87-5</t>
+  </si>
+  <si>
+    <t>120-12-7</t>
+  </si>
+  <si>
+    <t>56-55-3</t>
+  </si>
+  <si>
+    <t>50-32-8</t>
+  </si>
+  <si>
+    <t>207-08-9</t>
+  </si>
+  <si>
+    <t>218-01-9</t>
+  </si>
+  <si>
+    <t>206-44-0</t>
+  </si>
+  <si>
+    <t>91-20-3</t>
+  </si>
+  <si>
+    <t>129-00-0</t>
+  </si>
+  <si>
+    <t>105-67-9</t>
+  </si>
+  <si>
+    <t>99-76-3</t>
+  </si>
+  <si>
+    <t>21850-44-2</t>
+  </si>
+  <si>
+    <t>27581-13-1</t>
+  </si>
+  <si>
+    <t>59042-50-1</t>
+  </si>
+  <si>
+    <t>21245-02-3</t>
+  </si>
+  <si>
+    <t>80-05-7</t>
+  </si>
+  <si>
+    <t>94125-34-5</t>
+  </si>
+  <si>
+    <t>134-62-3</t>
+  </si>
+  <si>
+    <t>4376-20-9</t>
+  </si>
+  <si>
+    <t>75-27-4</t>
+  </si>
+  <si>
+    <t>2093-28-9</t>
+  </si>
+  <si>
+    <t>119-93-7</t>
+  </si>
+  <si>
+    <t>2008-41-5</t>
+  </si>
+  <si>
+    <t>2212-67-1</t>
+  </si>
+  <si>
+    <t>1929-77-7</t>
+  </si>
+  <si>
+    <t>105-54-4</t>
+  </si>
+  <si>
+    <t>16655-82-6</t>
+  </si>
+  <si>
+    <t>116-06-3</t>
+  </si>
+  <si>
+    <t>56-57-5</t>
+  </si>
+  <si>
+    <t>98-86-2</t>
+  </si>
+  <si>
+    <t>92-67-1</t>
+  </si>
+  <si>
+    <t>66-27-3</t>
+  </si>
+  <si>
+    <t>91-59-8</t>
+  </si>
+  <si>
+    <t>99-55-8</t>
+  </si>
+  <si>
+    <t>62-44-2</t>
+  </si>
+  <si>
+    <t>95-53-4</t>
+  </si>
+  <si>
+    <t>97-56-3</t>
+  </si>
+  <si>
+    <t>101-77-9</t>
+  </si>
+  <si>
+    <t>101-14-4</t>
+  </si>
+  <si>
+    <t>101-80-4</t>
+  </si>
+  <si>
+    <t>139-65-1</t>
+  </si>
+  <si>
+    <t>90-41-5</t>
+  </si>
+  <si>
+    <t>90-04-0</t>
+  </si>
+  <si>
+    <t>87-60-5</t>
+  </si>
+  <si>
+    <t>15299-99-7</t>
+  </si>
+  <si>
+    <t>56-81-5</t>
+  </si>
+  <si>
+    <t>14073-97-3</t>
+  </si>
+  <si>
+    <t>68359-37-5</t>
+  </si>
+  <si>
+    <t>91465-08-6</t>
+  </si>
+  <si>
+    <t>52315-07-8</t>
+  </si>
+  <si>
+    <t>51630-58-1</t>
+  </si>
+  <si>
+    <t>70124-77-5</t>
+  </si>
+  <si>
+    <t>10453-86-8</t>
+  </si>
+  <si>
+    <t>142-62-1</t>
+  </si>
+  <si>
+    <t>995-32-4</t>
+  </si>
+  <si>
+    <t>2355-31-9</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1427,7 +1648,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,30 +1995,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:Q1641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.6640625" customWidth="1"/>
-    <col min="12" max="12" width="142.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" customWidth="1"/>
+    <col min="13" max="13" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1807,34 +2029,37 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>2</v>
+        <v>420</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>73</v>
       </c>
@@ -1845,32 +2070,35 @@
         <v>217</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>5.75</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>6.0250000000000004</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>66</v>
       </c>
@@ -1881,32 +2109,35 @@
         <v>200</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>6.35</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>6.45</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>70</v>
       </c>
@@ -1917,32 +2148,35 @@
         <v>208</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>6.5750000000000002</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>6.7</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>76</v>
       </c>
@@ -1953,32 +2187,35 @@
         <v>224</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>7.05</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>7.25</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>67</v>
       </c>
@@ -1989,26 +2226,29 @@
         <v>201</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>79</v>
       </c>
@@ -2019,26 +2259,29 @@
         <v>230</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>68</v>
       </c>
@@ -2049,26 +2292,29 @@
         <v>204</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>69</v>
       </c>
@@ -2079,26 +2325,29 @@
         <v>207</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>80</v>
       </c>
@@ -2109,26 +2358,29 @@
         <v>232</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -2139,26 +2391,29 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -2169,26 +2424,29 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>4</v>
       </c>
@@ -2199,26 +2457,29 @@
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -2229,26 +2490,29 @@
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -2259,24 +2523,27 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -2287,26 +2554,29 @@
         <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>18</v>
       </c>
@@ -2317,26 +2587,29 @@
         <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>22</v>
       </c>
@@ -2347,26 +2620,29 @@
         <v>67</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>23</v>
       </c>
@@ -2377,26 +2653,29 @@
         <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>31</v>
       </c>
@@ -2407,24 +2686,27 @@
         <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>32</v>
       </c>
@@ -2435,26 +2717,29 @@
         <v>97</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44</v>
       </c>
@@ -2465,24 +2750,27 @@
         <v>132</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>46</v>
       </c>
@@ -2493,24 +2781,27 @@
         <v>137</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>50</v>
       </c>
@@ -2521,26 +2812,29 @@
         <v>149</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>52</v>
       </c>
@@ -2551,26 +2845,29 @@
         <v>155</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>53</v>
       </c>
@@ -2581,26 +2878,29 @@
         <v>158</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="2"/>
+      <c r="M26" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>57</v>
       </c>
@@ -2611,26 +2911,29 @@
         <v>169</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="2"/>
+      <c r="M27" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>61</v>
       </c>
@@ -2641,24 +2944,27 @@
         <v>180</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>63</v>
       </c>
@@ -2669,26 +2975,29 @@
         <v>186</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="2"/>
+      <c r="K29" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2" t="s">
+      <c r="L29" s="2"/>
+      <c r="M29" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>7</v>
       </c>
@@ -2699,30 +3008,33 @@
         <v>22</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>7.85</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>7.9249999999999998</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="K30" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2" t="s">
+      <c r="L30" s="2"/>
+      <c r="M30" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>37</v>
       </c>
@@ -2733,30 +3045,33 @@
         <v>112</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>4.3</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>4.45</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="K31" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>38</v>
       </c>
@@ -2767,30 +3082,33 @@
         <v>115</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>4.25</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>4.45</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="K32" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2" t="s">
+      <c r="L32" s="2"/>
+      <c r="M32" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>78</v>
       </c>
@@ -2801,30 +3119,33 @@
         <v>228</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>16.425000000000001</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>16.574999999999999</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="K33" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="2"/>
+      <c r="M33" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>13</v>
       </c>
@@ -2835,30 +3156,33 @@
         <v>41</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>13.425000000000001</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="2"/>
+      <c r="M34" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>17</v>
       </c>
@@ -2869,30 +3193,33 @@
         <v>53</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>13.425000000000001</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="K35" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2" t="s">
+      <c r="L35" s="2"/>
+      <c r="M35" s="2" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45</v>
       </c>
@@ -2903,30 +3230,33 @@
         <v>134</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>13.425000000000001</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>13.574999999999999</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="K36" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="2"/>
+      <c r="M36" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>58</v>
       </c>
@@ -2937,30 +3267,33 @@
         <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>5.05</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="K37" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2" t="s">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>14</v>
       </c>
@@ -2971,30 +3304,33 @@
         <v>44</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>20</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>20.2</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="K38" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="2"/>
+      <c r="M38" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>40</v>
       </c>
@@ -3005,30 +3341,33 @@
         <v>121</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>12.85</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>13.025</v>
       </c>
-      <c r="J39" s="8" t="s">
+      <c r="K39" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>16</v>
       </c>
@@ -3039,30 +3378,33 @@
         <v>50</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>5</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>5.2</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="K40" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>25</v>
       </c>
@@ -3073,30 +3415,33 @@
         <v>76</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>6.05</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>6.25</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="K41" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="2"/>
+      <c r="M41" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>28</v>
       </c>
@@ -3107,30 +3452,33 @@
         <v>85</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>11.9</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>12.2</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="K42" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2" t="s">
+      <c r="L42" s="2"/>
+      <c r="M42" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>6</v>
       </c>
@@ -3141,30 +3489,33 @@
         <v>19</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>6.3</v>
       </c>
-      <c r="I43" s="2">
+      <c r="J43" s="2">
         <v>6.6</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="K43" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2" t="s">
+      <c r="L43" s="2"/>
+      <c r="M43" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -3175,30 +3526,33 @@
         <v>124</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="7"/>
+      <c r="G44" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>4.3</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="K44" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2" t="s">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>71</v>
       </c>
@@ -3209,32 +3563,35 @@
         <v>211</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G45" s="3">
-        <v>2</v>
-      </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
+        <v>2</v>
+      </c>
+      <c r="I45" s="2">
         <v>7.4</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>7.55</v>
       </c>
-      <c r="J45" s="8" t="s">
+      <c r="K45" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>33</v>
       </c>
@@ -3245,34 +3602,37 @@
         <v>100</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G46" s="3">
-        <v>2</v>
-      </c>
-      <c r="H46" s="2">
+      <c r="H46" s="3">
+        <v>2</v>
+      </c>
+      <c r="I46" s="2">
         <v>19.45</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="K46" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="M46" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>39</v>
       </c>
@@ -3283,34 +3643,37 @@
         <v>118</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="3">
-        <v>1</v>
-      </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
+        <v>1</v>
+      </c>
+      <c r="I47" s="2">
         <v>11.05</v>
       </c>
-      <c r="I47" s="2">
+      <c r="J47" s="2">
         <v>11.25</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="K47" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>62</v>
       </c>
@@ -3321,32 +3684,35 @@
         <v>183</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G48" s="3">
-        <v>1</v>
-      </c>
-      <c r="H48" s="2">
+      <c r="H48" s="3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="2">
         <v>17.149999999999999</v>
       </c>
-      <c r="I48" s="2">
+      <c r="J48" s="2">
         <v>17.45</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="K48" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>74</v>
       </c>
@@ -3357,32 +3723,35 @@
         <v>219</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G49" s="3">
-        <v>2</v>
-      </c>
-      <c r="H49" s="2">
+      <c r="H49" s="3">
+        <v>2</v>
+      </c>
+      <c r="I49" s="2">
         <v>5.15</v>
       </c>
-      <c r="I49" s="2">
+      <c r="J49" s="2">
         <v>5.3</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="K49" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>75</v>
       </c>
@@ -3393,32 +3762,35 @@
         <v>221</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G50" s="3">
-        <v>2</v>
-      </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
+        <v>2</v>
+      </c>
+      <c r="I50" s="2">
         <v>12.7</v>
       </c>
-      <c r="I50" s="2">
+      <c r="J50" s="2">
         <v>12.875</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="K50" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>77</v>
       </c>
@@ -3429,32 +3801,35 @@
         <v>226</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G51" s="3">
-        <v>2</v>
-      </c>
-      <c r="H51" s="2">
+      <c r="H51" s="3">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2">
         <v>7.2</v>
       </c>
-      <c r="I51" s="2">
+      <c r="J51" s="2">
         <v>7.4</v>
       </c>
-      <c r="J51" s="8" t="s">
+      <c r="K51" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>65</v>
       </c>
@@ -3465,32 +3840,35 @@
         <v>199</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G52" s="3">
-        <v>1</v>
-      </c>
-      <c r="H52" s="2">
+      <c r="H52" s="3">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2">
         <v>6.35</v>
       </c>
-      <c r="I52" s="2">
+      <c r="J52" s="2">
         <v>6.45</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="K52" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>72</v>
       </c>
@@ -3501,32 +3879,35 @@
         <v>214</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G53" s="3">
-        <v>1</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="H53" s="3">
+        <v>1</v>
+      </c>
+      <c r="I53" s="2">
         <v>6.0724999999999998</v>
       </c>
-      <c r="I53" s="2">
+      <c r="J53" s="2">
         <v>6.25</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="K53" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>64</v>
       </c>
@@ -3537,34 +3918,37 @@
         <v>196</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G54" s="3">
-        <v>1</v>
-      </c>
-      <c r="H54" s="2">
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2">
         <v>6.4</v>
       </c>
-      <c r="I54" s="2">
+      <c r="J54" s="2">
         <v>6.55</v>
       </c>
-      <c r="J54" s="8" t="s">
+      <c r="K54" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="L54" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="M54" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>1</v>
       </c>
@@ -3575,34 +3959,37 @@
         <v>4</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="3">
-        <v>1</v>
-      </c>
-      <c r="H55" s="2">
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2">
         <v>7.9749999999999996</v>
       </c>
-      <c r="I55" s="2">
+      <c r="J55" s="2">
         <v>8.15</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="K55" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="L55" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="L55" s="2" t="s">
+      <c r="M55" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>8</v>
       </c>
@@ -3613,34 +4000,37 @@
         <v>25</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G56" s="3">
-        <v>2</v>
-      </c>
-      <c r="H56" s="2">
+      <c r="H56" s="3">
+        <v>2</v>
+      </c>
+      <c r="I56" s="2">
         <v>7.4</v>
       </c>
-      <c r="I56" s="2">
+      <c r="J56" s="2">
         <v>7.5250000000000004</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="K56" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="L56" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="M56" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>15</v>
       </c>
@@ -3651,34 +4041,37 @@
         <v>47</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G57" s="3">
-        <v>1</v>
-      </c>
-      <c r="H57" s="2">
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2">
         <v>13.725</v>
       </c>
-      <c r="I57" s="2">
+      <c r="J57" s="2">
         <v>13.85</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="K57" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="L57" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="M57" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>10</v>
       </c>
@@ -3689,34 +4082,37 @@
         <v>32</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G58" s="3">
-        <v>1</v>
-      </c>
-      <c r="H58" s="2">
+      <c r="H58" s="3">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2">
         <v>13.25</v>
       </c>
-      <c r="I58" s="2">
+      <c r="J58" s="2">
         <v>13.45</v>
       </c>
-      <c r="J58" s="8" t="s">
+      <c r="K58" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="L58" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="L58" s="2" t="s">
+      <c r="M58" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>20</v>
       </c>
@@ -3727,32 +4123,35 @@
         <v>62</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="3">
-        <v>1</v>
-      </c>
-      <c r="H59" s="2">
+      <c r="H59" s="3">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2">
         <v>6.35</v>
       </c>
-      <c r="I59" s="2">
+      <c r="J59" s="2">
         <v>6.5</v>
       </c>
-      <c r="J59" s="8" t="s">
+      <c r="K59" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="L59" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="L59" s="2"/>
-    </row>
-    <row r="60" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>21</v>
       </c>
@@ -3763,32 +4162,35 @@
         <v>65</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G60" s="3">
-        <v>1</v>
-      </c>
-      <c r="H60" s="2">
+      <c r="H60" s="3">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2">
         <v>6.375</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <v>6.5</v>
       </c>
-      <c r="J60" s="8" t="s">
+      <c r="K60" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="L60" s="2"/>
-    </row>
-    <row r="61" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>24</v>
       </c>
@@ -3799,32 +4201,35 @@
         <v>73</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G61" s="3">
-        <v>1</v>
-      </c>
-      <c r="H61" s="2">
+      <c r="H61" s="3">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2">
         <v>9.0500000000000007</v>
       </c>
-      <c r="I61" s="2">
+      <c r="J61" s="2">
         <v>9.2249999999999996</v>
       </c>
-      <c r="J61" s="8" t="s">
+      <c r="K61" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="L61" s="2"/>
-    </row>
-    <row r="62" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>26</v>
       </c>
@@ -3835,32 +4240,35 @@
         <v>79</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G62" s="3">
-        <v>1</v>
-      </c>
-      <c r="H62" s="2">
+      <c r="H62" s="3">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2">
         <v>9.5749999999999993</v>
       </c>
-      <c r="I62" s="2">
+      <c r="J62" s="2">
         <v>9.7750000000000004</v>
       </c>
-      <c r="J62" s="8" t="s">
+      <c r="K62" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="L62" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="L62" s="2"/>
-    </row>
-    <row r="63" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>27</v>
       </c>
@@ -3871,32 +4279,35 @@
         <v>82</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G63" s="3">
-        <v>1</v>
-      </c>
-      <c r="H63" s="2">
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
         <v>3.8</v>
       </c>
-      <c r="I63" s="2">
+      <c r="J63" s="2">
         <v>3.95</v>
       </c>
-      <c r="J63" s="8" t="s">
+      <c r="K63" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K63" s="2" t="s">
+      <c r="L63" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="L63" s="2"/>
-    </row>
-    <row r="64" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>29</v>
       </c>
@@ -3907,34 +4318,37 @@
         <v>88</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G64" s="3">
-        <v>1</v>
-      </c>
-      <c r="H64" s="2">
+      <c r="H64" s="3">
+        <v>1</v>
+      </c>
+      <c r="I64" s="2">
         <v>9.4</v>
       </c>
-      <c r="I64" s="2">
+      <c r="J64" s="2">
         <v>9.65</v>
       </c>
-      <c r="J64" s="8" t="s">
+      <c r="K64" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="M64" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>30</v>
       </c>
@@ -3945,34 +4359,37 @@
         <v>91</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G65" s="3">
-        <v>1</v>
-      </c>
-      <c r="H65" s="2">
+      <c r="H65" s="3">
+        <v>1</v>
+      </c>
+      <c r="I65" s="2">
         <v>11.2</v>
       </c>
-      <c r="I65" s="2">
+      <c r="J65" s="2">
         <v>11.3575</v>
       </c>
-      <c r="J65" s="8" t="s">
+      <c r="K65" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="L65" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="M65" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>34</v>
       </c>
@@ -3983,32 +4400,35 @@
         <v>103</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G66" s="3">
-        <v>1</v>
-      </c>
-      <c r="H66" s="2">
+      <c r="H66" s="3">
+        <v>1</v>
+      </c>
+      <c r="I66" s="2">
         <v>22.3</v>
       </c>
-      <c r="I66" s="2">
+      <c r="J66" s="2">
         <v>22.45</v>
       </c>
-      <c r="J66" s="8" t="s">
+      <c r="K66" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="L66" s="2"/>
-    </row>
-    <row r="67" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>35</v>
       </c>
@@ -4019,34 +4439,37 @@
         <v>106</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G67" s="3">
-        <v>1</v>
-      </c>
-      <c r="H67" s="2">
+      <c r="H67" s="3">
+        <v>1</v>
+      </c>
+      <c r="I67" s="2">
         <v>9.4499999999999993</v>
       </c>
-      <c r="I67" s="2">
+      <c r="J67" s="2">
         <v>9.65</v>
       </c>
-      <c r="J67" s="8" t="s">
+      <c r="K67" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K67" s="2" t="s">
+      <c r="L67" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="M67" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>36</v>
       </c>
@@ -4057,34 +4480,37 @@
         <v>109</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G68" s="3">
-        <v>1</v>
-      </c>
-      <c r="H68" s="2">
+      <c r="H68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="2">
         <v>9.35</v>
       </c>
-      <c r="I68" s="2">
+      <c r="J68" s="2">
         <v>9.5500000000000007</v>
       </c>
-      <c r="J68" s="8" t="s">
+      <c r="K68" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="L68" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>43</v>
       </c>
@@ -4095,32 +4521,35 @@
         <v>130</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G69" s="3">
-        <v>1</v>
-      </c>
-      <c r="H69" s="2">
+      <c r="H69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="2">
         <v>2.25</v>
       </c>
-      <c r="I69" s="2">
+      <c r="J69" s="2">
         <v>2.5</v>
       </c>
-      <c r="J69" s="8" t="s">
+      <c r="K69" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="L69" s="2"/>
-    </row>
-    <row r="70" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>47</v>
       </c>
@@ -4131,32 +4560,35 @@
         <v>140</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G70" s="3">
-        <v>1</v>
-      </c>
-      <c r="H70" s="2">
+      <c r="H70" s="3">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2">
         <v>18</v>
       </c>
-      <c r="I70" s="2">
+      <c r="J70" s="2">
         <v>18.149999999999999</v>
       </c>
-      <c r="J70" s="8" t="s">
+      <c r="K70" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="L70" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="L70" s="2"/>
-    </row>
-    <row r="71" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>48</v>
       </c>
@@ -4167,32 +4599,35 @@
         <v>143</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G71" s="3">
-        <v>1</v>
-      </c>
-      <c r="H71" s="2">
+      <c r="H71" s="3">
+        <v>1</v>
+      </c>
+      <c r="I71" s="2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I71" s="2">
+      <c r="J71" s="2">
         <v>10.102499999999999</v>
       </c>
-      <c r="J71" s="8" t="s">
+      <c r="K71" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K71" s="2" t="s">
+      <c r="L71" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="L71" s="2"/>
-    </row>
-    <row r="72" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>54</v>
       </c>
@@ -4203,32 +4638,35 @@
         <v>161</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G72" s="3">
-        <v>1</v>
-      </c>
-      <c r="H72" s="2">
+      <c r="H72" s="3">
+        <v>1</v>
+      </c>
+      <c r="I72" s="2">
         <v>7.7</v>
       </c>
-      <c r="I72" s="2">
+      <c r="J72" s="2">
         <v>7.875</v>
       </c>
-      <c r="J72" s="8" t="s">
+      <c r="K72" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="L72" s="2"/>
-    </row>
-    <row r="73" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>55</v>
       </c>
@@ -4239,32 +4677,35 @@
         <v>163</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G73" s="3">
-        <v>1</v>
-      </c>
-      <c r="H73" s="2">
+      <c r="H73" s="3">
+        <v>1</v>
+      </c>
+      <c r="I73" s="2">
         <v>6.6</v>
       </c>
-      <c r="I73" s="2">
+      <c r="J73" s="2">
         <v>6.75</v>
       </c>
-      <c r="J73" s="8" t="s">
+      <c r="K73" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="L73" s="2"/>
-    </row>
-    <row r="74" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>60</v>
       </c>
@@ -4275,32 +4716,35 @@
         <v>177</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G74" s="3">
-        <v>1</v>
-      </c>
-      <c r="H74" s="2">
+      <c r="H74" s="3">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I74" s="2">
+      <c r="J74" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J74" s="8" t="s">
+      <c r="K74" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="L74" s="2"/>
-    </row>
-    <row r="75" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>49</v>
       </c>
@@ -4310,35 +4754,38 @@
       <c r="C75" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G75" s="3">
-        <v>1</v>
-      </c>
-      <c r="H75" s="2">
+      <c r="H75" s="3">
+        <v>1</v>
+      </c>
+      <c r="I75" s="2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I75" s="2">
+      <c r="J75" s="2">
         <v>10.1</v>
       </c>
-      <c r="J75" s="8" t="s">
+      <c r="K75" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="M75" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>56</v>
       </c>
@@ -4349,34 +4796,37 @@
         <v>166</v>
       </c>
       <c r="D76" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G76" s="3">
-        <v>1</v>
-      </c>
-      <c r="H76" s="2">
+      <c r="H76" s="3">
+        <v>1</v>
+      </c>
+      <c r="I76" s="2">
         <v>19.399999999999999</v>
       </c>
-      <c r="I76" s="2">
+      <c r="J76" s="2">
         <v>19.7</v>
       </c>
-      <c r="J76" s="8" t="s">
+      <c r="K76" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="L76" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="M76" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>59</v>
       </c>
@@ -4387,34 +4837,37 @@
         <v>175</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G77" s="3">
-        <v>1</v>
-      </c>
-      <c r="H77" s="2">
+      <c r="H77" s="3">
+        <v>1</v>
+      </c>
+      <c r="I77" s="2">
         <v>17.8</v>
       </c>
-      <c r="I77" s="2">
+      <c r="J77" s="2">
         <v>18</v>
       </c>
-      <c r="J77" s="8" t="s">
+      <c r="K77" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="L77" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="M77" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>19</v>
       </c>
@@ -4425,32 +4878,35 @@
         <v>59</v>
       </c>
       <c r="D78" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G78" s="3">
-        <v>1</v>
-      </c>
-      <c r="H78" s="2">
+      <c r="H78" s="3">
+        <v>1</v>
+      </c>
+      <c r="I78" s="2">
         <v>19.3</v>
       </c>
-      <c r="I78" s="2">
+      <c r="J78" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="J78" s="8" t="s">
+      <c r="K78" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="L78" s="2"/>
-    </row>
-    <row r="79" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>42</v>
       </c>
@@ -4461,34 +4917,37 @@
         <v>127</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G79" s="3">
-        <v>1</v>
-      </c>
-      <c r="H79" s="2">
+      <c r="H79" s="3">
+        <v>1</v>
+      </c>
+      <c r="I79" s="2">
         <v>7.3</v>
       </c>
-      <c r="I79" s="2">
+      <c r="J79" s="2">
         <v>7.5</v>
       </c>
-      <c r="J79" s="8" t="s">
+      <c r="K79" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="L79" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="M79" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -4499,34 +4958,37 @@
         <v>16</v>
       </c>
       <c r="D80" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G80" s="3">
-        <v>2</v>
-      </c>
-      <c r="H80" s="2">
+      <c r="H80" s="3">
+        <v>2</v>
+      </c>
+      <c r="I80" s="2">
         <v>3.8250000000000002</v>
       </c>
-      <c r="I80" s="2">
+      <c r="J80" s="2">
         <v>3.9249999999999998</v>
       </c>
-      <c r="J80" s="8" t="s">
+      <c r="K80" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>51</v>
       </c>
@@ -4537,35 +4999,86 @@
         <v>152</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G81" s="3">
-        <v>2</v>
-      </c>
-      <c r="H81" s="2">
+      <c r="H81" s="3">
+        <v>2</v>
+      </c>
+      <c r="I81" s="2">
         <v>8.0500000000000007</v>
       </c>
-      <c r="I81" s="2">
+      <c r="J81" s="2">
         <v>8.35</v>
       </c>
-      <c r="J81" s="8" t="s">
+      <c r="K81" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="K81" s="2" t="s">
+      <c r="L81" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+    </row>
+    <row r="930" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q930" s="15"/>
+    </row>
+    <row r="931" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q931" s="15"/>
+    </row>
+    <row r="932" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q932" s="15"/>
+    </row>
+    <row r="933" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q933" s="15"/>
+    </row>
+    <row r="986" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q986" s="15"/>
+    </row>
+    <row r="987" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q987" s="15"/>
+    </row>
+    <row r="988" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q988" s="15"/>
+    </row>
+    <row r="989" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q989" s="15"/>
+    </row>
+    <row r="1598" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1598" s="15"/>
+    </row>
+    <row r="1599" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1599" s="15"/>
+    </row>
+    <row r="1600" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1600" s="15"/>
+    </row>
+    <row r="1601" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1601" s="15"/>
+    </row>
+    <row r="1638" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1638" s="15"/>
+    </row>
+    <row r="1639" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1639" s="15"/>
+    </row>
+    <row r="1640" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1640" s="15"/>
+    </row>
+    <row r="1641" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1641" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L81" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L81">
-      <sortCondition ref="J1:J81"/>
+  <autoFilter ref="A1:M81" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M81">
+      <sortCondition ref="K1:K81"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4574,6 +5087,422 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FA5D44-A496-8348-881B-63FA0B2DED6B}">
+  <dimension ref="A1:Q1569"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" customWidth="1"/>
+    <col min="13" max="13" width="45.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7.55</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>12.7</v>
+      </c>
+      <c r="J4" s="2">
+        <v>12.875</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6.35</v>
+      </c>
+      <c r="J6" s="2">
+        <v>6.45</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6.0724999999999998</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6.25</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>6.55</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7.9749999999999996</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8.15</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="858" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q858" s="15"/>
+    </row>
+    <row r="859" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q859" s="15"/>
+    </row>
+    <row r="860" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q860" s="15"/>
+    </row>
+    <row r="861" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q861" s="15"/>
+    </row>
+    <row r="914" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q914" s="15"/>
+    </row>
+    <row r="915" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q915" s="15"/>
+    </row>
+    <row r="916" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q916" s="15"/>
+    </row>
+    <row r="917" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q917" s="15"/>
+    </row>
+    <row r="1526" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1526" s="15"/>
+    </row>
+    <row r="1527" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1527" s="15"/>
+    </row>
+    <row r="1528" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1528" s="15"/>
+    </row>
+    <row r="1529" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1529" s="15"/>
+    </row>
+    <row r="1566" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1566" s="15"/>
+    </row>
+    <row r="1567" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1567" s="15"/>
+    </row>
+    <row r="1568" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1568" s="15"/>
+    </row>
+    <row r="1569" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q1569" s="15"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:M9" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M9">
+      <sortCondition ref="B1:B9"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5095E4-A4A5-664C-BDB6-270C422A8A43}">
   <dimension ref="A1:J92"/>
   <sheetViews>

</xml_diff>